<commit_message>
Dev count run 20251205
</commit_message>
<xml_diff>
--- a/dev-count-runs/scm_summary_20251205.xlsx
+++ b/dev-count-runs/scm_summary_20251205.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>SCM Report Summary</t>
   </si>
@@ -36,7 +36,7 @@
     <t>Time of report</t>
   </si>
   <si>
-    <t>9:55:25 AM</t>
+    <t>10:05:53 AM</t>
   </si>
   <si>
     <t>Total unique contributors across GitLab</t>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>j.totzek@gmail.com</t>
+  </si>
+  <si>
+    <t>Veracode Dev Count</t>
+  </si>
+  <si>
+    <t>dev-count@veracode.com</t>
   </si>
   <si>
     <t>julian-veracode/veracode</t>
@@ -523,7 +529,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>115</v>
@@ -551,7 +557,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -562,7 +568,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
@@ -593,18 +599,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -615,7 +621,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -626,7 +632,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -637,7 +643,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -648,7 +654,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -659,7 +665,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -670,12 +676,23 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>